<commit_message>
Add sample data to excel, implement get all Post from source
</commit_message>
<xml_diff>
--- a/Programing/daily-dev-clone/daily-dev-sample-data.xlsx
+++ b/Programing/daily-dev-clone/daily-dev-sample-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mr Tao\Desktop\daily dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mentorship-Program\Programing\daily-dev-clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E0AF76-ED75-4828-BF3C-979623CE5E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B1DDA2-C1DB-4817-98ED-D428317DCE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D6A6F0A-D793-4DDE-9861-B65F3553A9EE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
   <si>
     <t>Source</t>
   </si>
@@ -45,9 +45,6 @@
     <t>domain_name</t>
   </si>
   <si>
-    <t>thorben-janssen.com</t>
-  </si>
-  <si>
     <t>RssLink</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>source_id</t>
   </si>
   <si>
-    <t>https://thorben-janssen.com/ai-glossary-for-java-developers</t>
-  </si>
-  <si>
     <t>https://thorben-janssen.com/feed/</t>
   </si>
   <si>
@@ -105,27 +99,12 @@
     <t>#machine-learning</t>
   </si>
   <si>
-    <t>medium.com/@sumsourabh14</t>
-  </si>
-  <si>
     <t>RssLink_id</t>
   </si>
   <si>
-    <t>https://medium.com/@sumsourabh14/feed</t>
-  </si>
-  <si>
-    <t>https://medium.com/@sumsourabh14/how-i-use-chatgpt-as-a-frontend-developer-5-ways-0494d6f1ab54</t>
-  </si>
-  <si>
     <t>#chatgpt</t>
   </si>
   <si>
-    <t>#react</t>
-  </si>
-  <si>
-    <t>https://thorben-janssen.com/idclass-record/</t>
-  </si>
-  <si>
     <t>#jpa</t>
   </si>
   <si>
@@ -138,16 +117,178 @@
     <t>vuduchuy@gmail.com</t>
   </si>
   <si>
-    <t>trinhthanh112@gmail.com</t>
-  </si>
-  <si>
-    <t>nguyenquyet33@gmail.com</t>
-  </si>
-  <si>
     <t>User_Follow_Tag</t>
   </si>
   <si>
     <t>user_id</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/</t>
+  </si>
+  <si>
+    <t>https://vladmihalcea.com/feed/</t>
+  </si>
+  <si>
+    <t>https://vladmihalcea.com</t>
+  </si>
+  <si>
+    <t>https://thorben-janssen.com</t>
+  </si>
+  <si>
+    <t>High-Performance Java Persistence Newsletter, Issue 67</t>
+  </si>
+  <si>
+    <t>https://vladmihalcea.com/high-performance-java-persistence-newsletter-issue-67/</t>
+  </si>
+  <si>
+    <t>Eleven years of blogging</t>
+  </si>
+  <si>
+    <t>https://vladmihalcea.com/eleven-years-of-blogging/</t>
+  </si>
+  <si>
+    <t>Keyset Pagination with Spring Data WindowIterator</t>
+  </si>
+  <si>
+    <t>https://vladmihalcea.com/spring-data-windowiterator/</t>
+  </si>
+  <si>
+    <t>A beginner’s guide to Spring Data Envers</t>
+  </si>
+  <si>
+    <t>https://vladmihalcea.com/spring-data-envers/</t>
+  </si>
+  <si>
+    <t>Embeddable Inheritance with JPA and Hibernate</t>
+  </si>
+  <si>
+    <t>https://vladmihalcea.com/embeddable-inheritance-jpa-hibernate/</t>
+  </si>
+  <si>
+    <t>AI Glossary for Java Developers</t>
+  </si>
+  <si>
+    <t>https://thorben-janssen.com/ai-glossary-for-java-developers/</t>
+  </si>
+  <si>
+    <t>How to define a repository with Jakarta Data and Hibernate</t>
+  </si>
+  <si>
+    <t>https://thorben-janssen.com/jakarta-data-repository/</t>
+  </si>
+  <si>
+    <t>Getting Started with Jakarta Data and Hibernate</t>
+  </si>
+  <si>
+    <t>https://thorben-janssen.com/getting-started-with-jakarta-data/</t>
+  </si>
+  <si>
+    <t>Should your tests manage transactions?</t>
+  </si>
+  <si>
+    <t>https://thorben-janssen.com/should-your-tests-manage-transactions/</t>
+  </si>
+  <si>
+    <t>Giá xăng tăng vọt gần 1.300 đồng/lít</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/kinh-doanh/gia-xang-tang-vot-gan-1300-donglit-20241010115745150.htm</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/rss/kinh-doanh.rss</t>
+  </si>
+  <si>
+    <t>Đại gia Trương Gia Bình thưởng đậm nhân tài, FPT phá đỉnh lịch sử</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/kinh-doanh/dai-gia-truong-gia-binh-thuong-dam-nhan-tai-fpt-pha-dinh-lich-su-20241010134139601.htm</t>
+  </si>
+  <si>
+    <t>Việt Nam trở lại quỹ đạo tăng trưởng cao, FDI chạm mốc 25 tỷ USD</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/kinh-doanh/viet-nam-tro-lai-quy-dao-tang-truong-cao-fdi-cham-moc-25-ty-usd-20241010101225809.htm</t>
+  </si>
+  <si>
+    <t>Đến chơi nhà người yêu, thanh niên "tiện tay" trộm xe máy</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/phap-luat/den-choi-nha-nguoi-yeu-thanh-nien-tien-tay-trom-xe-may-20241010121830090.htm</t>
+  </si>
+  <si>
+    <t>Trợ giúp pháp lý cho nữ sinh lớp 8 bị xâm hại đến mang song thai</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/phap-luat/tro-giup-phap-ly-cho-nu-sinh-lop-8-bi-xam-hai-den-mang-song-thai-20241010115958901.htm</t>
+  </si>
+  <si>
+    <t>Bitexco nói về việc nhận hơn 15.700 tỷ đồng từ bà Trương Mỹ Lan</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/phap-luat/bitexco-noi-ve-viec-nhan-hon-15700-ty-dong-tu-ba-truong-my-lan-20241010103806765.htm</t>
+  </si>
+  <si>
+    <t>Hai ô tô của chủ trường tư tại Đắk Lắk bị xịt sơn khi đỗ ở vỉa hè</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/phap-luat/hai-o-to-cua-chu-truong-tu-tai-dak-lak-bi-xit-son-khi-do-o-via-he-20241010100854759.htm</t>
+  </si>
+  <si>
+    <t>Người đàn ông bán cháo lòng giả danh công an, lừa vợ chồng "Tú Ác" chạy án</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/phap-luat/nguoi-dan-ong-ban-chao-long-gia-danh-cong-an-lua-vo-chong-tu-ac-chay-an-20241010090632750.htm</t>
+  </si>
+  <si>
+    <t>https://dantri.com.vn/rss/phap-luat.rss</t>
+  </si>
+  <si>
+    <t>#hinh-su</t>
+  </si>
+  <si>
+    <t>#lua-dao</t>
+  </si>
+  <si>
+    <t>#xam-hai</t>
+  </si>
+  <si>
+    <t>#xang</t>
+  </si>
+  <si>
+    <t>#chung-khoang</t>
+  </si>
+  <si>
+    <t>#FDI</t>
+  </si>
+  <si>
+    <t>#trom-cap</t>
+  </si>
+  <si>
+    <t>nguyenxuantien@gmail.com</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>Kinh doanh</t>
+  </si>
+  <si>
+    <t>Pháp luật</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>artificial intelligence</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>pubDate</t>
   </si>
 </sst>
 </file>
@@ -200,7 +341,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +390,12 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -274,7 +421,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -285,8 +432,9 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
@@ -301,8 +449,14 @@
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="10"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
+    <cellStyle name="60% - Accent2" xfId="10" builtinId="36"/>
     <cellStyle name="60% - Accent3" xfId="4" builtinId="40"/>
     <cellStyle name="60% - Accent4" xfId="6" builtinId="44"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -624,367 +778,852 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450B20A7-B4E3-4408-BF73-741DE1BE179A}">
-  <dimension ref="F4:T38"/>
+  <dimension ref="F4:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="35.08984375" customWidth="1"/>
+    <col min="7" max="7" width="22.453125" customWidth="1"/>
     <col min="8" max="8" width="51.90625" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="17.7265625" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
     <col min="13" max="13" width="27.7265625" customWidth="1"/>
     <col min="16" max="16" width="12.1796875" customWidth="1"/>
+    <col min="18" max="18" width="19.7265625" customWidth="1"/>
+    <col min="19" max="19" width="16.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="6:18" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="6:18" x14ac:dyDescent="0.35">
       <c r="G6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="Q6" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="7" spans="6:18" x14ac:dyDescent="0.35">
       <c r="G7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>6</v>
+      <c r="J7" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="6:18" x14ac:dyDescent="0.35">
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>8</v>
+      <c r="H8" t="s">
+        <v>30</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>3</v>
+        <v>31</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="6:18" x14ac:dyDescent="0.35">
       <c r="G9">
         <v>2</v>
       </c>
-      <c r="H9" t="s">
-        <v>25</v>
+      <c r="H9" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="I9">
         <v>2</v>
       </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
       <c r="L9">
         <v>2</v>
       </c>
-      <c r="M9" t="s">
-        <v>23</v>
+      <c r="M9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10">
+        <v>3</v>
+      </c>
+      <c r="R10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="6:18" x14ac:dyDescent="0.35">
       <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M16" t="s">
+      <c r="I17" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="R16" t="s">
+      <c r="N17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="6:19" ht="15" x14ac:dyDescent="0.4">
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19" t="s">
+        <v>16</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20" t="s">
+        <v>17</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>3</v>
+      </c>
+      <c r="N21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>4</v>
+      </c>
+      <c r="R21" t="s">
+        <v>18</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>6</v>
+      </c>
+      <c r="R22" t="s">
+        <v>19</v>
+      </c>
+      <c r="S22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>7</v>
+      </c>
+      <c r="R23" t="s">
+        <v>20</v>
+      </c>
+      <c r="S23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>5</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>8</v>
+      </c>
+      <c r="R24" t="s">
+        <v>22</v>
+      </c>
+      <c r="S24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>5</v>
+      </c>
+      <c r="N25">
+        <v>10</v>
+      </c>
+      <c r="Q25">
+        <v>9</v>
+      </c>
+      <c r="R25" t="s">
+        <v>69</v>
+      </c>
+      <c r="S25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F26">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>6</v>
+      </c>
+      <c r="N26">
+        <v>6</v>
+      </c>
+      <c r="Q26">
+        <v>10</v>
+      </c>
+      <c r="R26" t="s">
+        <v>23</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <v>7</v>
+      </c>
+      <c r="N27">
+        <v>10</v>
+      </c>
+      <c r="Q27">
+        <v>11</v>
+      </c>
+      <c r="R27" t="s">
+        <v>70</v>
+      </c>
+      <c r="S27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F28">
+        <v>11</v>
+      </c>
+      <c r="G28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+      <c r="M28">
+        <v>8</v>
+      </c>
+      <c r="N28">
+        <v>10</v>
+      </c>
+      <c r="Q28">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="F17" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="R28" t="s">
+        <v>71</v>
+      </c>
+      <c r="S28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F29">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>56</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+      <c r="M29">
         <v>10</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="N29">
+        <v>13</v>
+      </c>
+      <c r="Q29">
+        <v>13</v>
+      </c>
+      <c r="R29" t="s">
+        <v>72</v>
+      </c>
+      <c r="S29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="I30" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="M30">
         <v>11</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="N30">
+        <v>14</v>
+      </c>
+      <c r="Q30">
+        <v>14</v>
+      </c>
+      <c r="R30" t="s">
+        <v>73</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F31">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="M31">
+        <v>12</v>
+      </c>
+      <c r="N31">
+        <v>15</v>
+      </c>
+      <c r="Q31">
+        <v>15</v>
+      </c>
+      <c r="R31" t="s">
+        <v>74</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F32">
+        <v>15</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="M32">
+        <v>13</v>
+      </c>
+      <c r="N32">
+        <v>9</v>
+      </c>
+      <c r="Q32">
+        <v>16</v>
+      </c>
+      <c r="R32" t="s">
+        <v>75</v>
+      </c>
+      <c r="S32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F33">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>13</v>
+      </c>
+      <c r="N33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="F34">
+        <v>17</v>
+      </c>
+      <c r="G34" t="s">
+        <v>66</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I34" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+      <c r="M34">
+        <v>14</v>
+      </c>
+      <c r="N34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="M35">
+        <v>15</v>
+      </c>
+      <c r="N35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="M36">
+        <v>16</v>
+      </c>
+      <c r="N36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="M37">
+        <v>17</v>
+      </c>
+      <c r="N37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="M38">
+        <v>17</v>
+      </c>
+      <c r="N38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N43" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="M17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="4" t="s">
+      <c r="R43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S44" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="6:20" ht="15" x14ac:dyDescent="0.4">
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="8">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="H19" s="10" t="s">
+    </row>
+    <row r="45" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>2</v>
-      </c>
-      <c r="R19">
-        <v>2</v>
-      </c>
-      <c r="S19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="F20">
-        <v>3</v>
-      </c>
-      <c r="H20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>5</v>
-      </c>
-      <c r="R20">
-        <v>3</v>
-      </c>
-      <c r="S20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>6</v>
-      </c>
-      <c r="R21">
-        <v>4</v>
-      </c>
-      <c r="S21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="M22">
-        <v>2</v>
-      </c>
-      <c r="N22">
-        <v>7</v>
-      </c>
-      <c r="R22">
-        <v>5</v>
-      </c>
-      <c r="S22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="M23">
-        <v>2</v>
-      </c>
-      <c r="N23">
-        <v>8</v>
-      </c>
-      <c r="R23">
-        <v>6</v>
-      </c>
-      <c r="S23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="M24">
-        <v>3</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="R24">
-        <v>7</v>
-      </c>
-      <c r="S24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="M25">
-        <v>3</v>
-      </c>
-      <c r="N25">
-        <v>2</v>
-      </c>
-      <c r="R25">
-        <v>8</v>
-      </c>
-      <c r="S25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="M26">
-        <v>3</v>
-      </c>
-      <c r="N26">
+      <c r="R45">
+        <v>1</v>
+      </c>
+      <c r="S45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="N46">
+        <v>2</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R46">
+        <v>1</v>
+      </c>
+      <c r="S46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="O47" s="3"/>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="S47">
         <v>9</v>
       </c>
-      <c r="R26">
-        <v>9</v>
-      </c>
-      <c r="S26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="L30" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="L31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q31" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="R31" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="L32">
-        <v>1</v>
-      </c>
-      <c r="M32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q32">
-        <v>1</v>
-      </c>
-      <c r="R32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="12:18" x14ac:dyDescent="0.35">
-      <c r="L33">
-        <v>2</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q33">
-        <v>1</v>
-      </c>
-      <c r="R33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="12:18" x14ac:dyDescent="0.35">
-      <c r="L34">
-        <v>3</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q34">
-        <v>1</v>
-      </c>
-      <c r="R34">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="12:18" x14ac:dyDescent="0.35">
-      <c r="Q35">
-        <v>2</v>
-      </c>
-      <c r="R35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="12:18" x14ac:dyDescent="0.35">
-      <c r="Q36">
-        <v>2</v>
-      </c>
-      <c r="R36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="12:18" x14ac:dyDescent="0.35">
-      <c r="Q37">
-        <v>3</v>
-      </c>
-      <c r="R37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="12:18" x14ac:dyDescent="0.35">
-      <c r="Q38">
-        <v>3</v>
-      </c>
-      <c r="R38">
-        <v>8</v>
+    </row>
+    <row r="48" spans="6:19" x14ac:dyDescent="0.35">
+      <c r="R48">
+        <v>1</v>
+      </c>
+      <c r="S48">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R49">
+        <v>1</v>
+      </c>
+      <c r="S49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R50">
+        <v>2</v>
+      </c>
+      <c r="S50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R51">
+        <v>2</v>
+      </c>
+      <c r="S51">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1001,11 +1640,31 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H19" r:id="rId1" xr:uid="{BF09219E-C1A7-487A-BDDF-4BDDF79525E3}"/>
-    <hyperlink ref="H8" r:id="rId2" xr:uid="{CDBDB158-7116-457B-BD1C-1C1B68F0D381}"/>
-    <hyperlink ref="M32" r:id="rId3" xr:uid="{F7C86750-57BD-44DC-BB53-41C535AA8005}"/>
-    <hyperlink ref="M33" r:id="rId4" xr:uid="{56D02AEF-67D1-4284-88D8-B50B91844C1A}"/>
-    <hyperlink ref="M34" r:id="rId5" xr:uid="{A0A28B16-CF4A-4C40-B28C-C7A2991BA91C}"/>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{CDBDB158-7116-457B-BD1C-1C1B68F0D381}"/>
+    <hyperlink ref="M8" r:id="rId2" xr:uid="{C5C3A605-6FD0-492E-996A-FD0B50090C70}"/>
+    <hyperlink ref="M9" r:id="rId3" xr:uid="{917C8FB0-FE85-4911-B2B2-98D4B0ACF280}"/>
+    <hyperlink ref="H19" r:id="rId4" xr:uid="{309617B6-DB8B-4A7F-8EF3-1D367D941238}"/>
+    <hyperlink ref="H20" r:id="rId5" xr:uid="{2695BD9B-C2AB-44C6-A5C8-7D738B9D2813}"/>
+    <hyperlink ref="H21" r:id="rId6" xr:uid="{38082DC1-9C67-4505-9906-800CC40C5841}"/>
+    <hyperlink ref="H22" r:id="rId7" xr:uid="{53D8C73F-CA12-4CA4-99D9-3B3C4CBD3119}"/>
+    <hyperlink ref="H18" r:id="rId8" xr:uid="{B6623B9D-FDEE-4C6A-972A-28FF43B93569}"/>
+    <hyperlink ref="H23" r:id="rId9" xr:uid="{4A86C6BF-BC47-489D-80C0-2961520067DA}"/>
+    <hyperlink ref="H24" r:id="rId10" xr:uid="{983F006B-16BB-47E7-BC54-06C2F73D9ADD}"/>
+    <hyperlink ref="H25" r:id="rId11" xr:uid="{3244F7FC-A3CB-4585-B054-77D1399F546A}"/>
+    <hyperlink ref="H26" r:id="rId12" xr:uid="{0B10A8E3-069B-47F5-9030-BE62FD702B12}"/>
+    <hyperlink ref="H27" r:id="rId13" xr:uid="{1671C4BA-6E61-4EA0-9AD4-174BF48E2462}"/>
+    <hyperlink ref="M10" r:id="rId14" xr:uid="{42CE399B-23A0-4E6F-AC81-F99D4542A2BB}"/>
+    <hyperlink ref="H10" r:id="rId15" xr:uid="{3B71BEDD-5520-4E11-8730-389E2E30467F}"/>
+    <hyperlink ref="H28" r:id="rId16" xr:uid="{07C21B9A-80CE-431D-9408-8E8CC9E4AF81}"/>
+    <hyperlink ref="H29" r:id="rId17" xr:uid="{67EB95C3-C83A-461D-8F91-34C79280D72D}"/>
+    <hyperlink ref="H30" r:id="rId18" xr:uid="{0C63D396-61F2-4476-B554-C30C50B55CD5}"/>
+    <hyperlink ref="H31" r:id="rId19" xr:uid="{E2931433-435C-467B-9954-E9A8A4F6828B}"/>
+    <hyperlink ref="H32" r:id="rId20" xr:uid="{2A6168E8-AC30-43A4-90CA-F5803F54F84C}"/>
+    <hyperlink ref="H33" r:id="rId21" xr:uid="{01D44D8B-2A96-4483-9682-258A3A5BCF9E}"/>
+    <hyperlink ref="H34" r:id="rId22" xr:uid="{606D7D54-FBDB-434B-9E48-3F8D08A51FB0}"/>
+    <hyperlink ref="H11" r:id="rId23" xr:uid="{3C83C4C4-584A-47EF-9C35-82FC1ADDE53B}"/>
+    <hyperlink ref="O45" r:id="rId24" xr:uid="{9CF62C41-9234-4F1D-949C-A3F2979C8A9E}"/>
+    <hyperlink ref="O46" r:id="rId25" xr:uid="{63C3559B-B587-46A2-9EB8-F7059D543B36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add sample data for comments, get comments from a post
</commit_message>
<xml_diff>
--- a/Programing/daily-dev-clone/daily-dev-sample-data.xlsx
+++ b/Programing/daily-dev-clone/daily-dev-sample-data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mentorship-Program\Programing\daily-dev-clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1429B7D4-E288-44A5-90DE-C6C065EAD14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52BF33A-4A77-4F9D-8E03-719F14345E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D6A6F0A-D793-4DDE-9861-B65F3553A9EE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8D6A6F0A-D793-4DDE-9861-B65F3553A9EE}"/>
   </bookViews>
   <sheets>
     <sheet name="User_Tag" sheetId="1" r:id="rId1"/>
+    <sheet name="comment in post" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
   <si>
     <t>Source</t>
   </si>
@@ -292,6 +293,39 @@
   </si>
   <si>
     <t>politic</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>hoangnguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>replied_comment_id</t>
+  </si>
+  <si>
+    <t>Cảm ơn bạn, bài viết rất dễ hiểu</t>
+  </si>
+  <si>
+    <t>Bạn có thể cho tôi xin sách tham khảo không</t>
+  </si>
+  <si>
+    <t>Tham khảo Jpa in Action</t>
+  </si>
+  <si>
+    <t>Cảm ơn bạn</t>
+  </si>
+  <si>
+    <t>Còn quyển nào khác không.</t>
+  </si>
+  <si>
+    <t>Tôi vẫn chưa hiểu phần thiết lập cho lắm</t>
   </si>
 </sst>
 </file>
@@ -783,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450B20A7-B4E3-4408-BF73-741DE1BE179A}">
   <dimension ref="F4:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView topLeftCell="C13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1679,4 +1713,356 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28FEBBE-7A19-43CF-8976-D02FEDCA2997}">
+  <dimension ref="C6:S27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="32.90625" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.6328125" customWidth="1"/>
+    <col min="7" max="7" width="20.26953125" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" customWidth="1"/>
+    <col min="11" max="11" width="26.90625" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" ht="15" x14ac:dyDescent="0.4">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <v>7</v>
+      </c>
+      <c r="J14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="14">
+        <v>45575.670601851853</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C20" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.35">
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{5E8AA609-643C-4AE4-AC70-F3E50BFA12AE}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{7764473E-7F24-44F7-8D95-B40F568DDDA3}"/>
+    <hyperlink ref="K9" r:id="rId3" xr:uid="{857C2832-E595-4E85-A00A-B36CEE854477}"/>
+    <hyperlink ref="K10" r:id="rId4" xr:uid="{E09C766F-6C0E-4BE0-9876-61E941306B13}"/>
+    <hyperlink ref="K11" r:id="rId5" xr:uid="{1893F8A6-5FF1-41A9-BCA2-0BE4181F8456}"/>
+    <hyperlink ref="K12" r:id="rId6" xr:uid="{80E48466-2FF9-42C8-BD41-707A69BBA41F}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{4453B0B9-C470-4597-8499-AF931601B497}"/>
+    <hyperlink ref="K13" r:id="rId8" xr:uid="{180F0C49-D199-470A-8F0A-5D4086EFA406}"/>
+    <hyperlink ref="K14" r:id="rId9" xr:uid="{AB4AE495-DBF0-4162-BAFA-0EE084885A57}"/>
+    <hyperlink ref="K15" r:id="rId10" xr:uid="{DD8CF9A9-C422-4269-BCC4-6126C2BC107C}"/>
+    <hyperlink ref="D10" r:id="rId11" xr:uid="{337A7AAC-1F60-4DAB-BC4B-D77EFA3A7C9E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>